<commit_message>
Daily attendance processing - 2025-09-29 21:42:51
</commit_message>
<xml_diff>
--- a/attendance_reports/Y3_B2526_CNS_session_analysis.xlsx
+++ b/attendance_reports/Y3_B2526_CNS_session_analysis.xlsx
@@ -1087,7 +1087,7 @@
       </c>
       <c r="G12" s="2" t="inlineStr">
         <is>
-          <t>wessam.atef@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg, Omnia.Mohammed@med.asu.edu.eg</t>
+          <t>wessam.atef@med.asu.edu.eg, Omnia.Mohammed@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H12" s="2" t="inlineStr">
@@ -2226,7 +2226,7 @@
       </c>
       <c r="G34" s="2" t="inlineStr">
         <is>
-          <t>wessam.atef@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg, Omnia.Mohammed@med.asu.edu.eg</t>
+          <t>wessam.atef@med.asu.edu.eg, Omnia.Mohammed@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H34" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2025-09-30 03:00:59
</commit_message>
<xml_diff>
--- a/attendance_reports/Y3_B2526_CNS_session_analysis.xlsx
+++ b/attendance_reports/Y3_B2526_CNS_session_analysis.xlsx
@@ -1086,7 +1086,7 @@
       </c>
       <c r="G12" s="6" t="inlineStr">
         <is>
-          <t>Omnia.Mohammed@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg, wessam.atef@med.asu.edu.eg</t>
+          <t>wessam.atef@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg, Omnia.Mohammed@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H12" s="6" t="inlineStr">
@@ -2221,7 +2221,7 @@
       </c>
       <c r="G34" s="6" t="inlineStr">
         <is>
-          <t>Omnia.Mohammed@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg, wessam.atef@med.asu.edu.eg</t>
+          <t>wessam.atef@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg, Omnia.Mohammed@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H34" s="6" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2025-09-30 03:29:21
</commit_message>
<xml_diff>
--- a/attendance_reports/Y3_B2526_CNS_session_analysis.xlsx
+++ b/attendance_reports/Y3_B2526_CNS_session_analysis.xlsx
@@ -1086,7 +1086,7 @@
       </c>
       <c r="G12" s="6" t="inlineStr">
         <is>
-          <t>wessam.atef@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg, Omnia.Mohammed@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>wessam.atef@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, Omnia.Mohammed@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H12" s="6" t="inlineStr">
@@ -2221,7 +2221,7 @@
       </c>
       <c r="G34" s="6" t="inlineStr">
         <is>
-          <t>wessam.atef@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg, Omnia.Mohammed@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>wessam.atef@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, Omnia.Mohammed@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H34" s="6" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2025-09-30 03:33:53
</commit_message>
<xml_diff>
--- a/attendance_reports/Y3_B2526_CNS_session_analysis.xlsx
+++ b/attendance_reports/Y3_B2526_CNS_session_analysis.xlsx
@@ -1086,7 +1086,7 @@
       </c>
       <c r="G12" s="6" t="inlineStr">
         <is>
-          <t>wessam.atef@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, Omnia.Mohammed@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg</t>
+          <t>wessam.atef@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg, Omnia.Mohammed@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H12" s="6" t="inlineStr">
@@ -2221,7 +2221,7 @@
       </c>
       <c r="G34" s="6" t="inlineStr">
         <is>
-          <t>wessam.atef@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, Omnia.Mohammed@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg</t>
+          <t>wessam.atef@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg, Omnia.Mohammed@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H34" s="6" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2025-09-30 07:15:03
</commit_message>
<xml_diff>
--- a/attendance_reports/Y3_B2526_CNS_session_analysis.xlsx
+++ b/attendance_reports/Y3_B2526_CNS_session_analysis.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Session Analysis Results" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Session Analysis Results" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1006,7 +1006,7 @@
       </c>
       <c r="L10" s="5" t="inlineStr">
         <is>
-          <t>3.9%</t>
+          <t>28.9%</t>
         </is>
       </c>
     </row>
@@ -1086,12 +1086,12 @@
       </c>
       <c r="G12" s="6" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, wessam.atef@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg</t>
+          <t>mariam.noureldin@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, Omnia.Mohammed@med.asu.edu.eg, wessam.atef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H12" s="6" t="inlineStr">
         <is>
-          <t>1/221</t>
+          <t>64/221</t>
         </is>
       </c>
       <c r="I12" s="6" t="inlineStr">
@@ -1310,7 +1310,7 @@
       </c>
       <c r="S15" s="5" t="inlineStr">
         <is>
-          <t>0.5%</t>
+          <t>29.0%</t>
         </is>
       </c>
     </row>
@@ -1388,7 +1388,7 @@
       </c>
       <c r="S16" s="5" t="inlineStr">
         <is>
-          <t>7.3%</t>
+          <t>28.9%</t>
         </is>
       </c>
     </row>
@@ -2221,12 +2221,12 @@
       </c>
       <c r="G34" s="6" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, wessam.atef@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg</t>
+          <t>mariam.noureldin@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, Omnia.Mohammed@med.asu.edu.eg, wessam.atef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H34" s="6" t="inlineStr">
         <is>
-          <t>18/246</t>
+          <t>71/246</t>
         </is>
       </c>
       <c r="I34" s="6" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2025-10-01 03:43:55
</commit_message>
<xml_diff>
--- a/attendance_reports/Y3_B2526_CNS_session_analysis.xlsx
+++ b/attendance_reports/Y3_B2526_CNS_session_analysis.xlsx
@@ -1090,7 +1090,7 @@
       </c>
       <c r="G12" s="4" t="inlineStr">
         <is>
-          <t>Omnia.Mohammed@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, wessam.atef@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg</t>
+          <t>Omnia.Mohammed@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg, wessam.atef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H12" s="4" t="inlineStr">
@@ -2229,7 +2229,7 @@
       </c>
       <c r="G34" s="4" t="inlineStr">
         <is>
-          <t>Omnia.Mohammed@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, wessam.atef@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg</t>
+          <t>Omnia.Mohammed@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg, wessam.atef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H34" s="4" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2025-10-01 07:58:49
</commit_message>
<xml_diff>
--- a/attendance_reports/Y3_B2526_CNS_session_analysis.xlsx
+++ b/attendance_reports/Y3_B2526_CNS_session_analysis.xlsx
@@ -1090,7 +1090,7 @@
       </c>
       <c r="G12" s="4" t="inlineStr">
         <is>
-          <t>Omnia.Mohammed@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg, wessam.atef@med.asu.edu.eg</t>
+          <t>Omnia.Mohammed@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg, wessam.atef@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H12" s="4" t="inlineStr">
@@ -2229,7 +2229,7 @@
       </c>
       <c r="G34" s="4" t="inlineStr">
         <is>
-          <t>Omnia.Mohammed@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg, wessam.atef@med.asu.edu.eg</t>
+          <t>Omnia.Mohammed@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg, wessam.atef@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H34" s="4" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2025-10-08 06:28:09
</commit_message>
<xml_diff>
--- a/attendance_reports/Y3_B2526_CNS_session_analysis.xlsx
+++ b/attendance_reports/Y3_B2526_CNS_session_analysis.xlsx
@@ -629,7 +629,7 @@
       </c>
       <c r="G3" s="4" t="inlineStr">
         <is>
-          <t>Amira.Sobhy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>eman.tantawi@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="4" t="inlineStr">
@@ -1090,7 +1090,7 @@
       </c>
       <c r="G12" s="4" t="inlineStr">
         <is>
-          <t>Omnia.Mohammed@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, wessam.atef@med.asu.edu.eg</t>
+          <t>mariam.noureldin@med.asu.edu.eg, wessam.atef@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, Omnia.Mohammed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H12" s="4" t="inlineStr">
@@ -1838,7 +1838,7 @@
       </c>
       <c r="G25" s="4" t="inlineStr">
         <is>
-          <t>Amira.Sobhy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>eman.tantawi@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H25" s="4" t="inlineStr">
@@ -2229,7 +2229,7 @@
       </c>
       <c r="G34" s="4" t="inlineStr">
         <is>
-          <t>Omnia.Mohammed@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, wessam.atef@med.asu.edu.eg</t>
+          <t>mariam.noureldin@med.asu.edu.eg, wessam.atef@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, Omnia.Mohammed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H34" s="4" t="inlineStr">
@@ -2534,7 +2534,7 @@
       </c>
       <c r="G41" s="4" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, ola.m.abdelfattah@med.asu.edu.eg, marina_atef@med.asu.edu.eg, wafaa.ebida@med.asu.edu.eg, Monica.Eshak@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, Salma.hassan@med.asu.edu.eg</t>
+          <t>youstina.magdy@med.asu.edu.eg, marina_atef@med.asu.edu.eg, wafaa.ebida@med.asu.edu.eg, Monica.Eshak@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, ola.m.abdelfattah@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg, Salma.hassan@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H41" s="4" t="inlineStr">

</xml_diff>